<commit_message>
impl.: is-script, add: online help to the main menu, set: default games dir., fix: mem-info, code-map
</commit_message>
<xml_diff>
--- a/Specification/!My/NESMemory.xlsx
+++ b/Specification/!My/NESMemory.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\artst\Documents\! My\Progects\! Programming\ASD\NESCore\Documents\Specification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\artst\Documents\! My\Progects\! Programming\ASD\ASD.NES\Specification\!My\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="Memory Map" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Memory Map'!$A$1:$K$57</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr autoRecover="0"/>
   <extLst>
@@ -489,7 +492,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -563,6 +566,13 @@
       <family val="3"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -789,7 +799,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -875,6 +885,87 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -882,99 +973,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1291,10 +1304,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:M59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55:J55"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1302,7 +1315,7 @@
     <col min="1" max="16384" width="10.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>148</v>
       </c>
@@ -1322,21 +1335,21 @@
       <c r="F1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="62" t="s">
+      <c r="G1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
       <c r="K1" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="43">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="30">
         <v>256</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="31"/>
       <c r="C2" s="6" t="s">
         <v>7</v>
       </c>
@@ -1349,21 +1362,21 @@
       <c r="F2" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="G2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="47"/>
-      <c r="I2" s="47"/>
-      <c r="J2" s="47"/>
-      <c r="K2" s="32" t="s">
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="62" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="33">
         <v>256</v>
       </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
@@ -1376,19 +1389,19 @@
       <c r="F3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="33"/>
-    </row>
-    <row r="4" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="35">
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="60"/>
+    </row>
+    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="47">
         <v>1536</v>
       </c>
-      <c r="B4" s="36"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1401,21 +1414,21 @@
       <c r="F4" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="49"/>
+      <c r="J4" s="49"/>
       <c r="K4" s="28" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="59">
+    <row r="5" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="36">
         <v>6144</v>
       </c>
-      <c r="B5" s="60"/>
+      <c r="B5" s="37"/>
       <c r="C5" s="4" t="s">
         <v>23</v>
       </c>
@@ -1426,211 +1439,212 @@
         <v>16</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="H5" s="61"/>
-      <c r="I5" s="61"/>
-      <c r="J5" s="61"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
       <c r="K5" s="21" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43">
-        <v>1</v>
-      </c>
-      <c r="B6" s="44"/>
+    <row r="6" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="30">
+        <v>1</v>
+      </c>
+      <c r="B6" s="31"/>
       <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="50"/>
+      <c r="E6" s="42"/>
       <c r="F6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="47" t="s">
+      <c r="G6" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="48" t="s">
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="59" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="38">
-        <v>1</v>
-      </c>
-      <c r="B7" s="39"/>
+    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="33">
+        <v>1</v>
+      </c>
+      <c r="B7" s="34"/>
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="52"/>
+      <c r="E7" s="44"/>
       <c r="F7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="33"/>
-    </row>
-    <row r="8" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="35">
-        <v>1</v>
-      </c>
-      <c r="B8" s="36"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="60"/>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="47">
+        <v>1</v>
+      </c>
+      <c r="B8" s="48"/>
       <c r="C8" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="53" t="s">
+      <c r="D8" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="54"/>
+      <c r="E8" s="46"/>
       <c r="F8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="34" t="s">
+      <c r="G8" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="37"/>
-    </row>
-    <row r="9" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43">
-        <v>1</v>
-      </c>
-      <c r="B9" s="44"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="61"/>
+    </row>
+    <row r="9" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="30">
+        <v>1</v>
+      </c>
+      <c r="B9" s="31"/>
       <c r="C9" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="50"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="47" t="s">
+      <c r="G9" s="32" t="s">
         <v>97</v>
       </c>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
-      <c r="J9" s="47"/>
-      <c r="K9" s="48" t="s">
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="59" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="35">
-        <v>1</v>
-      </c>
-      <c r="B10" s="36"/>
+      <c r="M9" s="63"/>
+    </row>
+    <row r="10" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="47">
+        <v>1</v>
+      </c>
+      <c r="B10" s="48"/>
       <c r="C10" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="53" t="s">
+      <c r="D10" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="E10" s="54"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="37"/>
-    </row>
-    <row r="11" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="43">
-        <v>1</v>
-      </c>
-      <c r="B11" s="44"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="49"/>
+      <c r="J10" s="49"/>
+      <c r="K10" s="61"/>
+    </row>
+    <row r="11" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30">
+        <v>1</v>
+      </c>
+      <c r="B11" s="31"/>
       <c r="C11" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="E11" s="50"/>
+      <c r="E11" s="42"/>
       <c r="F11" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G11" s="47" t="s">
+      <c r="G11" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="H11" s="47"/>
-      <c r="I11" s="47"/>
-      <c r="J11" s="47"/>
-      <c r="K11" s="48" t="s">
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="59" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38">
-        <v>1</v>
-      </c>
-      <c r="B12" s="39"/>
+    <row r="12" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="33">
+        <v>1</v>
+      </c>
+      <c r="B12" s="34"/>
       <c r="C12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="E12" s="52"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="33"/>
-    </row>
-    <row r="13" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="35">
-        <v>1</v>
-      </c>
-      <c r="B13" s="36"/>
+      <c r="H12" s="35"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="60"/>
+    </row>
+    <row r="13" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="47">
+        <v>1</v>
+      </c>
+      <c r="B13" s="48"/>
       <c r="C13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="53" t="s">
+      <c r="D13" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="54"/>
+      <c r="E13" s="46"/>
       <c r="F13" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="34" t="s">
+      <c r="G13" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="34"/>
-      <c r="K13" s="37"/>
-    </row>
-    <row r="14" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59">
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="61"/>
+    </row>
+    <row r="14" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36">
         <v>8184</v>
       </c>
-      <c r="B14" s="60"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="4" t="s">
         <v>22</v>
       </c>
@@ -1641,581 +1655,581 @@
         <v>21</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="61" t="s">
+      <c r="G14" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
       <c r="K14" s="22" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="43">
-        <v>1</v>
-      </c>
-      <c r="B15" s="44"/>
+    <row r="15" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="30">
+        <v>1</v>
+      </c>
+      <c r="B15" s="31"/>
       <c r="C15" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="46"/>
+      <c r="E15" s="40"/>
       <c r="F15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="47" t="s">
+      <c r="G15" s="32" t="s">
         <v>102</v>
       </c>
-      <c r="H15" s="47"/>
-      <c r="I15" s="47"/>
-      <c r="J15" s="47"/>
-      <c r="K15" s="32" t="s">
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="62" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="38">
-        <v>1</v>
-      </c>
-      <c r="B16" s="39"/>
+    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="33">
+        <v>1</v>
+      </c>
+      <c r="B16" s="34"/>
       <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D16" s="40" t="s">
+      <c r="D16" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="41"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="33"/>
+      <c r="H16" s="35"/>
+      <c r="I16" s="35"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="60"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="38">
-        <v>1</v>
-      </c>
-      <c r="B17" s="39"/>
+      <c r="A17" s="33">
+        <v>1</v>
+      </c>
+      <c r="B17" s="34"/>
       <c r="C17" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="D17" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="41"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G17" s="42" t="s">
+      <c r="G17" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
-      <c r="J17" s="42"/>
-      <c r="K17" s="33"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="60"/>
     </row>
     <row r="18" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38">
-        <v>1</v>
-      </c>
-      <c r="B18" s="39"/>
+      <c r="A18" s="33">
+        <v>1</v>
+      </c>
+      <c r="B18" s="34"/>
       <c r="C18" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="50" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="41"/>
+      <c r="E18" s="51"/>
       <c r="F18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G18" s="42" t="s">
+      <c r="G18" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="33"/>
+      <c r="H18" s="35"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="60"/>
     </row>
     <row r="19" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="38">
-        <v>1</v>
-      </c>
-      <c r="B19" s="39"/>
+      <c r="A19" s="33">
+        <v>1</v>
+      </c>
+      <c r="B19" s="34"/>
       <c r="C19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="E19" s="41"/>
+      <c r="E19" s="51"/>
       <c r="F19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="33"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="60"/>
     </row>
     <row r="20" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="38">
-        <v>1</v>
-      </c>
-      <c r="B20" s="39"/>
+      <c r="A20" s="33">
+        <v>1</v>
+      </c>
+      <c r="B20" s="34"/>
       <c r="C20" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="40" t="s">
+      <c r="D20" s="50" t="s">
         <v>32</v>
       </c>
-      <c r="E20" s="41"/>
+      <c r="E20" s="51"/>
       <c r="F20" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="33"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="60"/>
     </row>
     <row r="21" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="38">
-        <v>1</v>
-      </c>
-      <c r="B21" s="39"/>
+      <c r="A21" s="33">
+        <v>1</v>
+      </c>
+      <c r="B21" s="34"/>
       <c r="C21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="40" t="s">
+      <c r="D21" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="E21" s="41"/>
+      <c r="E21" s="51"/>
       <c r="F21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G21" s="42" t="s">
+      <c r="G21" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="33"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="60"/>
     </row>
     <row r="22" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="38">
-        <v>1</v>
-      </c>
-      <c r="B22" s="39"/>
+      <c r="A22" s="33">
+        <v>1</v>
+      </c>
+      <c r="B22" s="34"/>
       <c r="C22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D22" s="40" t="s">
+      <c r="D22" s="50" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="41"/>
+      <c r="E22" s="51"/>
       <c r="F22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="42" t="s">
+      <c r="G22" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="33"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="60"/>
     </row>
     <row r="23" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="38">
-        <v>1</v>
-      </c>
-      <c r="B23" s="39"/>
+      <c r="A23" s="33">
+        <v>1</v>
+      </c>
+      <c r="B23" s="34"/>
       <c r="C23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="D23" s="50" t="s">
         <v>35</v>
       </c>
-      <c r="E23" s="41"/>
+      <c r="E23" s="51"/>
       <c r="F23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G23" s="42" t="s">
+      <c r="G23" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="33"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="60"/>
     </row>
     <row r="24" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38">
-        <v>1</v>
-      </c>
-      <c r="B24" s="39"/>
+      <c r="A24" s="33">
+        <v>1</v>
+      </c>
+      <c r="B24" s="34"/>
       <c r="C24" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="40" t="s">
+      <c r="D24" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="41"/>
+      <c r="E24" s="51"/>
       <c r="F24" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G24" s="42" t="s">
+      <c r="G24" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="33"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="60"/>
     </row>
     <row r="25" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="38">
-        <v>1</v>
-      </c>
-      <c r="B25" s="39"/>
+      <c r="A25" s="33">
+        <v>1</v>
+      </c>
+      <c r="B25" s="34"/>
       <c r="C25" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="40" t="s">
+      <c r="D25" s="50" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="41"/>
+      <c r="E25" s="51"/>
       <c r="F25" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G25" s="42" t="s">
+      <c r="G25" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="33"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="60"/>
     </row>
     <row r="26" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="38">
-        <v>1</v>
-      </c>
-      <c r="B26" s="39"/>
+      <c r="A26" s="33">
+        <v>1</v>
+      </c>
+      <c r="B26" s="34"/>
       <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="40" t="s">
+      <c r="D26" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="41"/>
+      <c r="E26" s="51"/>
       <c r="F26" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G26" s="42" t="s">
+      <c r="G26" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="33"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="60"/>
     </row>
     <row r="27" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="38">
-        <v>1</v>
-      </c>
-      <c r="B27" s="39"/>
+      <c r="A27" s="33">
+        <v>1</v>
+      </c>
+      <c r="B27" s="34"/>
       <c r="C27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="40" t="s">
+      <c r="D27" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="E27" s="41"/>
+      <c r="E27" s="51"/>
       <c r="F27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G27" s="42" t="s">
+      <c r="G27" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="33"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="60"/>
     </row>
     <row r="28" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="38">
-        <v>1</v>
-      </c>
-      <c r="B28" s="39"/>
+      <c r="A28" s="33">
+        <v>1</v>
+      </c>
+      <c r="B28" s="34"/>
       <c r="C28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D28" s="40" t="s">
+      <c r="D28" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="41"/>
+      <c r="E28" s="51"/>
       <c r="F28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G28" s="42" t="s">
+      <c r="G28" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="33"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="60"/>
     </row>
     <row r="29" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="38">
-        <v>1</v>
-      </c>
-      <c r="B29" s="39"/>
+      <c r="A29" s="33">
+        <v>1</v>
+      </c>
+      <c r="B29" s="34"/>
       <c r="C29" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="40" t="s">
+      <c r="D29" s="50" t="s">
         <v>50</v>
       </c>
-      <c r="E29" s="41"/>
+      <c r="E29" s="51"/>
       <c r="F29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G29" s="42" t="s">
+      <c r="G29" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="H29" s="42"/>
-      <c r="I29" s="42"/>
-      <c r="J29" s="42"/>
-      <c r="K29" s="33"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="60"/>
     </row>
     <row r="30" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="38">
-        <v>1</v>
-      </c>
-      <c r="B30" s="39"/>
+      <c r="A30" s="33">
+        <v>1</v>
+      </c>
+      <c r="B30" s="34"/>
       <c r="C30" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D30" s="40" t="s">
+      <c r="D30" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="E30" s="41"/>
+      <c r="E30" s="51"/>
       <c r="F30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G30" s="42" t="s">
+      <c r="G30" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="H30" s="42"/>
-      <c r="I30" s="42"/>
-      <c r="J30" s="42"/>
-      <c r="K30" s="33"/>
+      <c r="H30" s="35"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="60"/>
     </row>
     <row r="31" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="38">
-        <v>1</v>
-      </c>
-      <c r="B31" s="39"/>
+      <c r="A31" s="33">
+        <v>1</v>
+      </c>
+      <c r="B31" s="34"/>
       <c r="C31" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="40" t="s">
+      <c r="D31" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="E31" s="41"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G31" s="42" t="s">
+      <c r="G31" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="H31" s="42"/>
-      <c r="I31" s="42"/>
-      <c r="J31" s="42"/>
-      <c r="K31" s="33"/>
+      <c r="H31" s="35"/>
+      <c r="I31" s="35"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="60"/>
     </row>
     <row r="32" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38">
-        <v>1</v>
-      </c>
-      <c r="B32" s="39"/>
+      <c r="A32" s="33">
+        <v>1</v>
+      </c>
+      <c r="B32" s="34"/>
       <c r="C32" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="40" t="s">
+      <c r="D32" s="50" t="s">
         <v>38</v>
       </c>
-      <c r="E32" s="41"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G32" s="42" t="s">
+      <c r="G32" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="H32" s="42"/>
-      <c r="I32" s="42"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="33"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="35"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="60"/>
     </row>
     <row r="33" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="38">
-        <v>1</v>
-      </c>
-      <c r="B33" s="39"/>
+      <c r="A33" s="33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="34"/>
       <c r="C33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D33" s="40" t="s">
+      <c r="D33" s="50" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="41"/>
+      <c r="E33" s="51"/>
       <c r="F33" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G33" s="42" t="s">
+      <c r="G33" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="H33" s="42"/>
-      <c r="I33" s="42"/>
-      <c r="J33" s="42"/>
-      <c r="K33" s="33"/>
+      <c r="H33" s="35"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="60"/>
     </row>
     <row r="34" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="35">
-        <v>1</v>
-      </c>
-      <c r="B34" s="36"/>
+      <c r="A34" s="47">
+        <v>1</v>
+      </c>
+      <c r="B34" s="48"/>
       <c r="C34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D34" s="55" t="s">
+      <c r="D34" s="54" t="s">
         <v>40</v>
       </c>
-      <c r="E34" s="56"/>
+      <c r="E34" s="55"/>
       <c r="F34" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G34" s="34" t="s">
+      <c r="G34" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="H34" s="34"/>
-      <c r="I34" s="34"/>
-      <c r="J34" s="34"/>
-      <c r="K34" s="37"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="61"/>
     </row>
     <row r="35" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29">
-        <v>1</v>
-      </c>
-      <c r="B35" s="30"/>
+      <c r="A35" s="56">
+        <v>1</v>
+      </c>
+      <c r="B35" s="57"/>
       <c r="C35" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D35" s="57" t="s">
+      <c r="D35" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="E35" s="58"/>
+      <c r="E35" s="53"/>
       <c r="F35" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="58" t="s">
         <v>67</v>
       </c>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
+      <c r="H35" s="58"/>
+      <c r="I35" s="58"/>
+      <c r="J35" s="58"/>
       <c r="K35" s="23" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29">
-        <v>1</v>
-      </c>
-      <c r="B36" s="30"/>
+      <c r="A36" s="56">
+        <v>1</v>
+      </c>
+      <c r="B36" s="57"/>
       <c r="C36" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D36" s="57" t="s">
+      <c r="D36" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="58"/>
+      <c r="E36" s="53"/>
       <c r="F36" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="58" t="s">
         <v>121</v>
       </c>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
+      <c r="H36" s="58"/>
+      <c r="I36" s="58"/>
+      <c r="J36" s="58"/>
       <c r="K36" s="23" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="37" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="43">
-        <v>1</v>
-      </c>
-      <c r="B37" s="44"/>
+      <c r="A37" s="30">
+        <v>1</v>
+      </c>
+      <c r="B37" s="31"/>
       <c r="C37" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D37" s="45" t="s">
+      <c r="D37" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="46"/>
+      <c r="E37" s="40"/>
       <c r="F37" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G37" s="47" t="s">
+      <c r="G37" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="H37" s="47"/>
-      <c r="I37" s="47"/>
-      <c r="J37" s="47"/>
-      <c r="K37" s="32" t="s">
+      <c r="H37" s="32"/>
+      <c r="I37" s="32"/>
+      <c r="J37" s="32"/>
+      <c r="K37" s="62" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="35">
-        <v>1</v>
-      </c>
-      <c r="B38" s="36"/>
+      <c r="A38" s="47">
+        <v>1</v>
+      </c>
+      <c r="B38" s="48"/>
       <c r="C38" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="55" t="s">
+      <c r="D38" s="54" t="s">
         <v>44</v>
       </c>
-      <c r="E38" s="56"/>
+      <c r="E38" s="55"/>
       <c r="F38" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G38" s="34" t="s">
+      <c r="G38" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="37"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="61"/>
     </row>
     <row r="39" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="29">
+      <c r="A39" s="56">
         <v>8</v>
       </c>
-      <c r="B39" s="30"/>
+      <c r="B39" s="57"/>
       <c r="C39" s="5" t="s">
         <v>19</v>
       </c>
@@ -2228,182 +2242,182 @@
       <c r="F39" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="H39" s="31"/>
-      <c r="I39" s="31"/>
-      <c r="J39" s="31"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="58"/>
+      <c r="J39" s="58"/>
       <c r="K39" s="24"/>
     </row>
     <row r="40" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="43">
-        <v>1</v>
-      </c>
-      <c r="B40" s="44"/>
+      <c r="A40" s="30">
+        <v>1</v>
+      </c>
+      <c r="B40" s="31"/>
       <c r="C40" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D40" s="45" t="s">
+      <c r="D40" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="46"/>
+      <c r="E40" s="40"/>
       <c r="F40" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G40" s="47" t="s">
+      <c r="G40" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="H40" s="47"/>
-      <c r="I40" s="47"/>
-      <c r="J40" s="47"/>
-      <c r="K40" s="32" t="s">
+      <c r="H40" s="32"/>
+      <c r="I40" s="32"/>
+      <c r="J40" s="32"/>
+      <c r="K40" s="62" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="38">
-        <v>1</v>
-      </c>
-      <c r="B41" s="39"/>
+      <c r="A41" s="33">
+        <v>1</v>
+      </c>
+      <c r="B41" s="34"/>
       <c r="C41" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D41" s="40" t="s">
+      <c r="D41" s="50" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="41"/>
+      <c r="E41" s="51"/>
       <c r="F41" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G41" s="42" t="s">
+      <c r="G41" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="H41" s="42"/>
-      <c r="I41" s="42"/>
-      <c r="J41" s="42"/>
-      <c r="K41" s="33"/>
+      <c r="H41" s="35"/>
+      <c r="I41" s="35"/>
+      <c r="J41" s="35"/>
+      <c r="K41" s="60"/>
     </row>
     <row r="42" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="38">
-        <v>1</v>
-      </c>
-      <c r="B42" s="39"/>
+      <c r="A42" s="33">
+        <v>1</v>
+      </c>
+      <c r="B42" s="34"/>
       <c r="C42" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D42" s="40" t="s">
+      <c r="D42" s="50" t="s">
         <v>81</v>
       </c>
-      <c r="E42" s="41"/>
+      <c r="E42" s="51"/>
       <c r="F42" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G42" s="42" t="s">
+      <c r="G42" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="H42" s="42"/>
-      <c r="I42" s="42"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="33"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="60"/>
     </row>
     <row r="43" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="38">
-        <v>1</v>
-      </c>
-      <c r="B43" s="39"/>
+      <c r="A43" s="33">
+        <v>1</v>
+      </c>
+      <c r="B43" s="34"/>
       <c r="C43" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D43" s="50" t="s">
         <v>82</v>
       </c>
-      <c r="E43" s="41"/>
+      <c r="E43" s="51"/>
       <c r="F43" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G43" s="42" t="s">
+      <c r="G43" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H43" s="42"/>
-      <c r="I43" s="42"/>
-      <c r="J43" s="42"/>
-      <c r="K43" s="33"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="60"/>
     </row>
     <row r="44" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="38">
-        <v>1</v>
-      </c>
-      <c r="B44" s="39"/>
+      <c r="A44" s="33">
+        <v>1</v>
+      </c>
+      <c r="B44" s="34"/>
       <c r="C44" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D44" s="40" t="s">
+      <c r="D44" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="E44" s="41"/>
+      <c r="E44" s="51"/>
       <c r="F44" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G44" s="42" t="s">
+      <c r="G44" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="H44" s="42"/>
-      <c r="I44" s="42"/>
-      <c r="J44" s="42"/>
-      <c r="K44" s="33"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="60"/>
     </row>
     <row r="45" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="38">
-        <v>1</v>
-      </c>
-      <c r="B45" s="39"/>
+      <c r="A45" s="33">
+        <v>1</v>
+      </c>
+      <c r="B45" s="34"/>
       <c r="C45" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D45" s="40" t="s">
+      <c r="D45" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="E45" s="41"/>
+      <c r="E45" s="51"/>
       <c r="F45" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G45" s="42" t="s">
+      <c r="G45" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="H45" s="42"/>
-      <c r="I45" s="42"/>
-      <c r="J45" s="42"/>
-      <c r="K45" s="33"/>
+      <c r="H45" s="35"/>
+      <c r="I45" s="35"/>
+      <c r="J45" s="35"/>
+      <c r="K45" s="60"/>
     </row>
     <row r="46" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="38">
-        <v>1</v>
-      </c>
-      <c r="B46" s="39"/>
+      <c r="A46" s="33">
+        <v>1</v>
+      </c>
+      <c r="B46" s="34"/>
       <c r="C46" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D46" s="40" t="s">
+      <c r="D46" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="E46" s="41"/>
+      <c r="E46" s="51"/>
       <c r="F46" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G46" s="42" t="s">
+      <c r="G46" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="33"/>
+      <c r="H46" s="35"/>
+      <c r="I46" s="35"/>
+      <c r="J46" s="35"/>
+      <c r="K46" s="60"/>
     </row>
     <row r="47" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="38">
+      <c r="A47" s="33">
         <v>9</v>
       </c>
-      <c r="B47" s="39"/>
+      <c r="B47" s="34"/>
       <c r="C47" s="2" t="s">
         <v>30</v>
       </c>
@@ -2416,111 +2430,111 @@
       <c r="F47" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G47" s="42" t="s">
+      <c r="G47" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="H47" s="42"/>
-      <c r="I47" s="42"/>
-      <c r="J47" s="42"/>
-      <c r="K47" s="33"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="35"/>
+      <c r="J47" s="35"/>
+      <c r="K47" s="60"/>
     </row>
     <row r="48" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="38">
-        <v>1</v>
-      </c>
-      <c r="B48" s="39"/>
+      <c r="A48" s="33">
+        <v>1</v>
+      </c>
+      <c r="B48" s="34"/>
       <c r="C48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="D48" s="50" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="41"/>
+      <c r="E48" s="51"/>
       <c r="F48" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G48" s="42" t="s">
+      <c r="G48" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="H48" s="42"/>
-      <c r="I48" s="42"/>
-      <c r="J48" s="42"/>
-      <c r="K48" s="33"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="60"/>
     </row>
     <row r="49" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="38">
-        <v>1</v>
-      </c>
-      <c r="B49" s="39"/>
+      <c r="A49" s="33">
+        <v>1</v>
+      </c>
+      <c r="B49" s="34"/>
       <c r="C49" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="40" t="s">
+      <c r="D49" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="E49" s="41"/>
+      <c r="E49" s="51"/>
       <c r="F49" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G49" s="42" t="s">
+      <c r="G49" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="H49" s="42"/>
-      <c r="I49" s="42"/>
-      <c r="J49" s="42"/>
-      <c r="K49" s="33"/>
+      <c r="H49" s="35"/>
+      <c r="I49" s="35"/>
+      <c r="J49" s="35"/>
+      <c r="K49" s="60"/>
     </row>
     <row r="50" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="38">
-        <v>1</v>
-      </c>
-      <c r="B50" s="39"/>
+      <c r="A50" s="33">
+        <v>1</v>
+      </c>
+      <c r="B50" s="34"/>
       <c r="C50" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="D50" s="50" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="41"/>
+      <c r="E50" s="51"/>
       <c r="F50" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G50" s="42" t="s">
+      <c r="G50" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="H50" s="42"/>
-      <c r="I50" s="42"/>
-      <c r="J50" s="42"/>
-      <c r="K50" s="33"/>
+      <c r="H50" s="35"/>
+      <c r="I50" s="35"/>
+      <c r="J50" s="35"/>
+      <c r="K50" s="60"/>
     </row>
     <row r="51" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="38">
-        <v>1</v>
-      </c>
-      <c r="B51" s="39"/>
+      <c r="A51" s="33">
+        <v>1</v>
+      </c>
+      <c r="B51" s="34"/>
       <c r="C51" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D51" s="40" t="s">
+      <c r="D51" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="E51" s="41"/>
+      <c r="E51" s="51"/>
       <c r="F51" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="G51" s="42" t="s">
+      <c r="G51" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="H51" s="42"/>
-      <c r="I51" s="42"/>
-      <c r="J51" s="42"/>
-      <c r="K51" s="33"/>
+      <c r="H51" s="35"/>
+      <c r="I51" s="35"/>
+      <c r="J51" s="35"/>
+      <c r="K51" s="60"/>
     </row>
     <row r="52" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="35">
+      <c r="A52" s="47">
         <v>204</v>
       </c>
-      <c r="B52" s="36"/>
+      <c r="B52" s="48"/>
       <c r="C52" s="3" t="s">
         <v>130</v>
       </c>
@@ -2533,19 +2547,19 @@
       <c r="F52" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G52" s="34" t="s">
+      <c r="G52" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="H52" s="34"/>
-      <c r="I52" s="34"/>
-      <c r="J52" s="34"/>
-      <c r="K52" s="37"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="49"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="61"/>
     </row>
     <row r="53" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="29">
+      <c r="A53" s="56">
         <v>3840</v>
       </c>
-      <c r="B53" s="30"/>
+      <c r="B53" s="57"/>
       <c r="C53" s="5" t="s">
         <v>133</v>
       </c>
@@ -2558,19 +2572,19 @@
       <c r="F53" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="G53" s="31" t="s">
+      <c r="G53" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="H53" s="31"/>
-      <c r="I53" s="31"/>
-      <c r="J53" s="31"/>
+      <c r="H53" s="58"/>
+      <c r="I53" s="58"/>
+      <c r="J53" s="58"/>
       <c r="K53" s="23"/>
     </row>
     <row r="54" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="29">
+      <c r="A54" s="56">
         <v>4096</v>
       </c>
-      <c r="B54" s="30"/>
+      <c r="B54" s="57"/>
       <c r="C54" s="5" t="s">
         <v>136</v>
       </c>
@@ -2583,21 +2597,21 @@
       <c r="F54" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G54" s="31" t="s">
+      <c r="G54" s="58" t="s">
         <v>144</v>
       </c>
-      <c r="H54" s="31"/>
-      <c r="I54" s="31"/>
-      <c r="J54" s="31"/>
+      <c r="H54" s="58"/>
+      <c r="I54" s="58"/>
+      <c r="J54" s="58"/>
       <c r="K54" s="23" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="29">
+      <c r="A55" s="56">
         <v>8192</v>
       </c>
-      <c r="B55" s="30"/>
+      <c r="B55" s="57"/>
       <c r="C55" s="5" t="s">
         <v>17</v>
       </c>
@@ -2610,21 +2624,21 @@
       <c r="F55" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G55" s="31" t="s">
+      <c r="G55" s="58" t="s">
         <v>150</v>
       </c>
-      <c r="H55" s="31"/>
-      <c r="I55" s="31"/>
-      <c r="J55" s="31"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="58"/>
+      <c r="J55" s="58"/>
       <c r="K55" s="23" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="29">
+      <c r="A56" s="56">
         <v>16384</v>
       </c>
-      <c r="B56" s="30"/>
+      <c r="B56" s="57"/>
       <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
@@ -2637,21 +2651,21 @@
       <c r="F56" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G56" s="31" t="s">
+      <c r="G56" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="H56" s="31"/>
-      <c r="I56" s="31"/>
-      <c r="J56" s="31"/>
+      <c r="H56" s="58"/>
+      <c r="I56" s="58"/>
+      <c r="J56" s="58"/>
       <c r="K56" s="23" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="29">
+      <c r="A57" s="56">
         <v>16384</v>
       </c>
-      <c r="B57" s="30"/>
+      <c r="B57" s="57"/>
       <c r="C57" s="5" t="s">
         <v>24</v>
       </c>
@@ -2664,12 +2678,12 @@
       <c r="F57" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G57" s="31" t="s">
+      <c r="G57" s="58" t="s">
         <v>151</v>
       </c>
-      <c r="H57" s="31"/>
-      <c r="I57" s="31"/>
-      <c r="J57" s="31"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="58"/>
+      <c r="J57" s="58"/>
       <c r="K57" s="23" t="s">
         <v>146</v>
       </c>
@@ -2679,49 +2693,95 @@
     </row>
   </sheetData>
   <mergeCells count="163">
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="G2:J2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="G3:J3"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="G15:J15"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="G4:J4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G5:J5"/>
-    <mergeCell ref="G16:J16"/>
-    <mergeCell ref="G17:J17"/>
-    <mergeCell ref="G18:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="G57:J57"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="G54:J54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="G55:J55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="G56:J56"/>
+    <mergeCell ref="G52:J52"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="K40:K52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="G53:J53"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="G50:J50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="G51:J51"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="G43:J43"/>
+    <mergeCell ref="G48:J48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="G49:J49"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="G47:J47"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="G44:J44"/>
+    <mergeCell ref="G45:J45"/>
+    <mergeCell ref="G46:J46"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="G40:J40"/>
+    <mergeCell ref="G41:J41"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="G39:J39"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="G26:J26"/>
+    <mergeCell ref="G27:J27"/>
+    <mergeCell ref="G28:J28"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="G30:J30"/>
+    <mergeCell ref="G31:J31"/>
+    <mergeCell ref="G42:J42"/>
+    <mergeCell ref="K6:K8"/>
+    <mergeCell ref="K9:K10"/>
+    <mergeCell ref="K11:K13"/>
+    <mergeCell ref="K15:K34"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G10:J10"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="G12:J12"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="G37:J37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="G38:J38"/>
+    <mergeCell ref="G32:J32"/>
+    <mergeCell ref="G33:J33"/>
+    <mergeCell ref="G34:J34"/>
+    <mergeCell ref="G35:J35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="G36:J36"/>
     <mergeCell ref="D35:E35"/>
     <mergeCell ref="D24:E24"/>
     <mergeCell ref="A24:B24"/>
@@ -2746,104 +2806,59 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="D25:E25"/>
     <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="G16:J16"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="G18:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="G2:J2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="G3:J3"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="G15:J15"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="G4:J4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G5:J5"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="D10:E10"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="G37:J37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="G38:J38"/>
-    <mergeCell ref="G32:J32"/>
-    <mergeCell ref="G33:J33"/>
-    <mergeCell ref="G34:J34"/>
-    <mergeCell ref="G35:J35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="G36:J36"/>
-    <mergeCell ref="G26:J26"/>
-    <mergeCell ref="G27:J27"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="G30:J30"/>
-    <mergeCell ref="G31:J31"/>
-    <mergeCell ref="G42:J42"/>
-    <mergeCell ref="K6:K8"/>
-    <mergeCell ref="K9:K10"/>
-    <mergeCell ref="K11:K13"/>
-    <mergeCell ref="K15:K34"/>
-    <mergeCell ref="K37:K38"/>
     <mergeCell ref="A13:B13"/>
-    <mergeCell ref="G7:J7"/>
-    <mergeCell ref="G8:J8"/>
-    <mergeCell ref="G9:J9"/>
-    <mergeCell ref="G10:J10"/>
-    <mergeCell ref="G11:J11"/>
-    <mergeCell ref="G12:J12"/>
-    <mergeCell ref="G13:J13"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="G39:J39"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="G49:J49"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="G47:J47"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="G44:J44"/>
-    <mergeCell ref="G45:J45"/>
-    <mergeCell ref="G46:J46"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="G40:J40"/>
-    <mergeCell ref="G41:J41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="G57:J57"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="G54:J54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="G55:J55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="G56:J56"/>
-    <mergeCell ref="G52:J52"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="K40:K52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="G53:J53"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="G50:J50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="G51:J51"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="G43:J43"/>
-    <mergeCell ref="G48:J48"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <printOptions horizontalCentered="1" verticalCentered="1"/>
+  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageSetup scale="83" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>